<commit_message>
Version up to v4.4.1
</commit_message>
<xml_diff>
--- a/docs/assets/InterProcessPyObjects/Throughput.xlsx
+++ b/docs/assets/InterProcessPyObjects/Throughput.xlsx
@@ -8,26 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40bbff9fbc1c97b1/Документи/Dev/Cengal/InterProcessPyObjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="233" documentId="8_{F8FFA07D-33F1-4D65-A7CA-6E4EDBBC1C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{802D440C-FAC8-4138-B27C-B69D085C4153}"/>
+  <xr:revisionPtr revIDLastSave="427" documentId="8_{F8FFA07D-33F1-4D65-A7CA-6E4EDBBC1C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D52CA6DA-730A-4E26-AA9B-A7D36EC629A5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="29760" windowHeight="17496" xr2:uid="{37BE1A55-5939-4F19-B03E-F319840E1CE8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="29760" windowHeight="17496" activeTab="2" xr2:uid="{37BE1A55-5939-4F19-B03E-F319840E1CE8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Throughput" sheetId="1" r:id="rId1"/>
+    <sheet name="Shared Dict" sheetId="2" r:id="rId2"/>
+    <sheet name="Shared Dict - 2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$17</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$F$2:$F$17</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$17</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$17</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$2:$D$17</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$2:$E$17</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$F$1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Approach</t>
   </si>
@@ -116,6 +105,51 @@
   <si>
     <t>multiprocessing.shared_memory (sync) *</t>
   </si>
+  <si>
+    <t>UltraDict</t>
+  </si>
+  <si>
+    <t>shared_memory_dict</t>
+  </si>
+  <si>
+    <t>increments/s</t>
+  </si>
+  <si>
+    <t>InterProcessPyObjects - Dict</t>
+  </si>
+  <si>
+    <t>multiprocessing.Manager - dict</t>
+  </si>
+  <si>
+    <t>InterProcessPyObjects - Dataclass</t>
+  </si>
+  <si>
+    <t>third-party-increments/s</t>
+  </si>
+  <si>
+    <t>own-increments/s</t>
+  </si>
+  <si>
+    <t>InterProcessPyObjects - IntEnumListStruct</t>
+  </si>
+  <si>
+    <t>players_num</t>
+  </si>
+  <si>
+    <t>iterations_num</t>
+  </si>
+  <si>
+    <t>sub_iterations_num</t>
+  </si>
+  <si>
+    <t>Third-party value_increments/s</t>
+  </si>
+  <si>
+    <t>InterProcessPyObjects value_increments/s</t>
+  </si>
+  <si>
+    <t>value_increments/s</t>
+  </si>
 </sst>
 </file>
 
@@ -124,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,16 +166,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -149,19 +197,161 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
@@ -181,6 +371,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDEA900"/>
+      <color rgb="FFE6AF00"/>
       <color rgb="FF008A0D"/>
     </mruColors>
   </colors>
@@ -221,7 +413,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Throughput!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -310,11 +502,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$2:$A$17</c15:sqref>
+                    <c15:sqref>Throughput!$A$2:$A$17</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$2,Sheet1!$A$4,Sheet1!$A$6,Sheet1!$A$8:$A$15)</c:f>
+              <c:f>(Throughput!$A$2,Throughput!$A$4,Throughput!$A$6,Throughput!$A$8:$A$15)</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -358,11 +550,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$E$2:$E$17</c15:sqref>
+                    <c15:sqref>Throughput!$E$2:$E$17</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$E$2,Sheet1!$E$4,Sheet1!$E$6,Sheet1!$E$8:$E$15)</c:f>
+              <c:f>(Throughput!$E$2,Throughput!$E$4,Throughput!$E$6,Throughput!$E$8:$E$15)</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
@@ -392,7 +584,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Throughput!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -479,11 +671,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$2:$A$17</c15:sqref>
+                    <c15:sqref>Throughput!$A$2:$A$17</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$2,Sheet1!$A$4,Sheet1!$A$6,Sheet1!$A$8:$A$15)</c:f>
+              <c:f>(Throughput!$A$2,Throughput!$A$4,Throughput!$A$6,Throughput!$A$8:$A$15)</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -527,11 +719,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$F$2:$F$17</c15:sqref>
+                    <c15:sqref>Throughput!$F$2:$F$17</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$F$2,Sheet1!$F$4,Sheet1!$F$6,Sheet1!$F$8:$F$15)</c:f>
+              <c:f>(Throughput!$F$2,Throughput!$F$4,Throughput!$F$6,Throughput!$F$8:$F$15)</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
@@ -589,7 +781,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$1</c15:sqref>
+                          <c15:sqref>Throughput!$B$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -680,10 +872,10 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$2:$A$17</c15:sqref>
+                          <c15:sqref>Throughput!$A$2:$A$17</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$2,Sheet1!$A$4,Sheet1!$A$6,Sheet1!$A$8:$A$15)</c15:sqref>
+                          <c15:sqref>(Throughput!$A$2,Throughput!$A$4,Throughput!$A$6,Throughput!$A$8:$A$15)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -730,10 +922,10 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$B$2:$B$17</c15:sqref>
+                          <c15:sqref>Throughput!$B$2:$B$17</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$B$2,Sheet1!$B$4,Sheet1!$B$6,Sheet1!$B$8:$B$15)</c15:sqref>
+                          <c15:sqref>(Throughput!$B$2,Throughput!$B$4,Throughput!$B$6,Throughput!$B$8:$B$15)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -792,7 +984,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$1</c15:sqref>
+                          <c15:sqref>Throughput!$C$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -883,10 +1075,10 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$2:$A$17</c15:sqref>
+                          <c15:sqref>Throughput!$A$2:$A$17</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$2,Sheet1!$A$4,Sheet1!$A$6,Sheet1!$A$8:$A$15)</c15:sqref>
+                          <c15:sqref>(Throughput!$A$2,Throughput!$A$4,Throughput!$A$6,Throughput!$A$8:$A$15)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -933,10 +1125,10 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$C$2:$C$17</c15:sqref>
+                          <c15:sqref>Throughput!$C$2:$C$17</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$C$2,Sheet1!$C$4,Sheet1!$C$6,Sheet1!$C$8:$C$15)</c15:sqref>
+                          <c15:sqref>(Throughput!$C$2,Throughput!$C$4,Throughput!$C$6,Throughput!$C$8:$C$15)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -995,7 +1187,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$D$1</c15:sqref>
+                          <c15:sqref>Throughput!$D$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1063,7 +1255,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -1087,10 +1279,10 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$2:$A$17</c15:sqref>
+                          <c15:sqref>Throughput!$A$2:$A$17</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$2,Sheet1!$A$4,Sheet1!$A$6,Sheet1!$A$8:$A$15)</c15:sqref>
+                          <c15:sqref>(Throughput!$A$2,Throughput!$A$4,Throughput!$A$6,Throughput!$A$8:$A$15)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1137,10 +1329,10 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$D$2:$D$17</c15:sqref>
+                          <c15:sqref>Throughput!$D$2:$D$17</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$D$2,Sheet1!$D$4,Sheet1!$D$6,Sheet1!$D$8:$D$15)</c15:sqref>
+                          <c15:sqref>(Throughput!$D$2,Throughput!$D$4,Throughput!$D$6,Throughput!$D$8:$D$15)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1183,7 +1375,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-2251-4CFA-8121-1DBF90946302}"/>
                   </c:ext>
@@ -1413,6 +1605,1408 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Shared Dict'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>third-party-increments/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Shared Dict'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>InterProcessPyObjects - IntEnumListStruct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>InterProcessPyObjects - Dataclass</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UltraDict</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shared_memory_dict</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>InterProcessPyObjects - Dict</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>multiprocessing.Manager - dict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Shared Dict'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="2">
+                  <c:v>92102.826735690702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50613.656070507001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1942.3214943963001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6C2B-4C42-B746-17D56908F969}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Shared Dict'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>own-increments/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="DEA900"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:srgbClr val="FFC000">
+                  <a:alpha val="25000"/>
+                </a:srgbClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Shared Dict'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>InterProcessPyObjects - IntEnumListStruct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>InterProcessPyObjects - Dataclass</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UltraDict</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shared_memory_dict</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>InterProcessPyObjects - Dict</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>multiprocessing.Manager - dict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Shared Dict'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1071404.2837357901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140799.736055374</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43155.413311345597</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6C2B-4C42-B746-17D56908F969}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="315"/>
+        <c:overlap val="100"/>
+        <c:axId val="1372874383"/>
+        <c:axId val="1378223087"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Shared Dict'!$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>increments/s</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:noFill/>
+                  <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:miter lim="800000"/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="63500">
+                      <a:schemeClr val="accent3">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="25000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="75000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Shared Dict'!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>InterProcessPyObjects - IntEnumListStruct</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>InterProcessPyObjects - Dataclass</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>UltraDict</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>shared_memory_dict</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>InterProcessPyObjects - Dict</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>multiprocessing.Manager - dict</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Shared Dict'!$D$2:$D$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>1071404.2837357901</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>140799.736055374</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>92102.826735690702</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>50613.656070507001</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>43155.413311345597</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1942.3214943963001</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-6C2B-4C42-B746-17D56908F969}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1372874383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1378223087"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1378223087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1372874383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr rot="0" vert="horz"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Shared Dict - 2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Third-party value_increments/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Shared Dict - 2'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>InterProcessPyObjects - IntEnumListStruct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>InterProcessPyObjects - Dataclass</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UltraDict</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>InterProcessPyObjects - Dict</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>shared_memory_dict</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>multiprocessing.Manager - dict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Shared Dict - 2'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="2">
+                  <c:v>76214.313856519497</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42861.6945536434</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2751.1005385550702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E1BB-4310-9B6E-28D27AB02D57}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Shared Dict - 2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>InterProcessPyObjects value_increments/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="DEA900"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:srgbClr val="FFC000">
+                  <a:alpha val="25000"/>
+                </a:srgbClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Shared Dict - 2'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>InterProcessPyObjects - IntEnumListStruct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>InterProcessPyObjects - Dataclass</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UltraDict</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>InterProcessPyObjects - Dict</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>shared_memory_dict</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>multiprocessing.Manager - dict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Shared Dict - 2'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1189729.9471072999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>143090.62753517399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44284.941270658899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E1BB-4310-9B6E-28D27AB02D57}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="315"/>
+        <c:overlap val="100"/>
+        <c:axId val="1372874383"/>
+        <c:axId val="1378223087"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Shared Dict - 2'!$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>value_increments/s</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:noFill/>
+                  <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                    <a:solidFill>
+                      <a:srgbClr val="DEA900"/>
+                    </a:solidFill>
+                    <a:miter lim="800000"/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="63500">
+                      <a:schemeClr val="accent3">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="25000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="75000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Shared Dict - 2'!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>InterProcessPyObjects - IntEnumListStruct</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>InterProcessPyObjects - Dataclass</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>UltraDict</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>InterProcessPyObjects - Dict</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>shared_memory_dict</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>multiprocessing.Manager - dict</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Shared Dict - 2'!$D$2:$D$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>1189729.9471072999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>143090.62753517399</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>76214.313856519497</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44284.941270658899</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>42861.6945536434</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2751.1005385550702</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-E1BB-4310-9B6E-28D27AB02D57}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1372874383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1378223087"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1378223087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1372874383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr rot="0" vert="horz"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1453,7 +3047,1185 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2043,6 +4815,92 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{777652A1-37D1-46AE-92CE-E5D8CA84F680}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF48107A-C7F5-4417-9108-A35A0054F164}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00C9A79F-48AE-4E7E-A44C-B0F853A26CE0}" name="Table1" displayName="Table1" ref="A1:F17" totalsRowShown="0">
   <autoFilter ref="A1:F17" xr:uid="{00C9A79F-48AE-4E7E-A44C-B0F853A26CE0}"/>
@@ -2051,19 +4909,55 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A01A263A-3A1C-4CFD-A15A-529A8FEAF477}" name="Approach"/>
-    <tableColumn id="2" xr3:uid="{BE933F3C-4BAE-47B1-A1A5-33A3968A17EB}" name="Throughput bytes/s" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{20DE3D9E-3235-49CF-9875-88CAA114E9D2}" name="Throughput MiB/s" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{BE933F3C-4BAE-47B1-A1A5-33A3968A17EB}" name="Throughput bytes/s" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{20DE3D9E-3235-49CF-9875-88CAA114E9D2}" name="Throughput MiB/s" dataDxfId="9">
       <calculatedColumnFormula>B2/(1024*1024)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CC33C0A5-B28F-4FBE-A02C-C5D8E85EB5C1}" name="Throughput GiB/s" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{CC33C0A5-B28F-4FBE-A02C-C5D8E85EB5C1}" name="Throughput GiB/s" dataDxfId="8">
       <calculatedColumnFormula>C2/1024</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC923873-9D64-45D2-87B8-CD4FEEACDE98}" name="Throughput GiB/s (sync)" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{FC923873-9D64-45D2-87B8-CD4FEEACDE98}" name="Throughput GiB/s (sync)" dataDxfId="7">
       <calculatedColumnFormula>C2/1024</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{50888BA8-5F35-4D7A-907B-60DE75E7E9A4}" name="Throughput GiB/s (async)" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{50888BA8-5F35-4D7A-907B-60DE75E7E9A4}" name="Throughput GiB/s (async)" dataDxfId="6">
       <calculatedColumnFormula>D3</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A566397-156C-4EC0-AF6D-3DAB26B13DA2}" name="Table13" displayName="Table13" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{9A566397-156C-4EC0-AF6D-3DAB26B13DA2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D7">
+    <sortCondition descending="1" ref="D1:D7"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{661A3131-E881-4917-82DB-18B4C1195F4F}" name="Approach"/>
+    <tableColumn id="2" xr3:uid="{982FA720-7A09-4426-AB1A-4AE408ACD463}" name="third-party-increments/s" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{4DDF94A8-1D45-4780-8C6E-E196C05B8D51}" name="own-increments/s" dataDxfId="4">
+      <calculatedColumnFormula>B2/(1024*1024)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{75560960-FEB1-4E1A-AF36-D132D65E2722}" name="increments/s" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7E9CD1D-1080-4563-BC02-55A4B02644DF}" name="Table134" displayName="Table134" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{C7E9CD1D-1080-4563-BC02-55A4B02644DF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D7">
+    <sortCondition descending="1" ref="D1:D7"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C47640D3-6EB6-44A1-B2AC-E8D0FA0E5B7B}" name="Approach"/>
+    <tableColumn id="2" xr3:uid="{1B386850-45BE-42F4-B8F2-B4D3BD2FA4AF}" name="Third-party value_increments/s" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E41F78BD-3D7D-4B15-9072-081720A2EB98}" name="InterProcessPyObjects value_increments/s" dataDxfId="1">
+      <calculatedColumnFormula>B2/(1024*1024)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{B5FBBE33-6989-4CA2-886F-68AB1FD65D99}" name="value_increments/s" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2388,8 +5282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90F4FF9-3E45-4916-8981-4C3D260284D2}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2431,11 +5325,11 @@
         <v>4048201349.4699998</v>
       </c>
       <c r="C2" s="2">
-        <f>B2/(1024*1024)</f>
+        <f t="shared" ref="C2:C15" si="0">B2/(1024*1024)</f>
         <v>3860.6656546306608</v>
       </c>
       <c r="D2" s="2">
-        <f>C2/1024</f>
+        <f t="shared" ref="D2:D15" si="1">C2/1024</f>
         <v>3.7701813033502547</v>
       </c>
       <c r="E2" s="2">
@@ -2452,11 +5346,11 @@
         <v>4048201349.4699998</v>
       </c>
       <c r="C3" s="2">
-        <f>B3/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>3860.6656546306608</v>
       </c>
       <c r="D3" s="2">
-        <f>C3/1024</f>
+        <f t="shared" si="1"/>
         <v>3.7701813033502547</v>
       </c>
       <c r="E3" s="2">
@@ -2473,11 +5367,11 @@
         <v>3460033553.8000002</v>
       </c>
       <c r="C4" s="2">
-        <f>B4/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>3299.745134162903</v>
       </c>
       <c r="D4" s="2">
-        <f>C4/1024</f>
+        <f t="shared" si="1"/>
         <v>3.22240735758096</v>
       </c>
       <c r="F4" s="2">
@@ -2493,11 +5387,11 @@
         <v>3460033553.8000002</v>
       </c>
       <c r="C5" s="2">
-        <f>B5/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>3299.745134162903</v>
       </c>
       <c r="D5" s="2">
-        <f>C5/1024</f>
+        <f t="shared" si="1"/>
         <v>3.22240735758096</v>
       </c>
       <c r="F5" s="2">
@@ -2513,11 +5407,11 @@
         <v>3306263028.23</v>
       </c>
       <c r="C6" s="2">
-        <f>B6/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>3153.0981333065033</v>
       </c>
       <c r="D6" s="2">
-        <f>C6/1024</f>
+        <f t="shared" si="1"/>
         <v>3.0791973958071321</v>
       </c>
       <c r="F6" s="2">
@@ -2533,11 +5427,11 @@
         <v>3306263028.23</v>
       </c>
       <c r="C7" s="2">
-        <f>B7/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>3153.0981333065033</v>
       </c>
       <c r="D7" s="2">
-        <f>C7/1024</f>
+        <f t="shared" si="1"/>
         <v>3.0791973958071321</v>
       </c>
       <c r="F7" s="2">
@@ -2553,11 +5447,11 @@
         <v>2882551472.7800002</v>
       </c>
       <c r="C8" s="2">
-        <f>B8/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>2749.0153053092959</v>
       </c>
       <c r="D8" s="2">
-        <f>C8/1024</f>
+        <f t="shared" si="1"/>
         <v>2.6845852590911092</v>
       </c>
       <c r="E8" s="2">
@@ -2574,11 +5468,11 @@
         <v>1036982532.75</v>
       </c>
       <c r="C9" s="2">
-        <f>B9/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>988.943608045578</v>
       </c>
       <c r="D9" s="2">
-        <f>C9/1024</f>
+        <f t="shared" si="1"/>
         <v>0.96576524223200977</v>
       </c>
       <c r="F9" s="2">
@@ -2594,11 +5488,11 @@
         <v>1011447292.65</v>
       </c>
       <c r="C10" s="2">
-        <f>B10/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>964.59130539894102</v>
       </c>
       <c r="D10" s="2">
-        <f>C10/1024</f>
+        <f t="shared" si="1"/>
         <v>0.94198369667865334</v>
       </c>
       <c r="F10" s="2">
@@ -2614,11 +5508,11 @@
         <v>990485364.95000005</v>
       </c>
       <c r="C11" s="2">
-        <f>B11/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>944.60045332908635</v>
       </c>
       <c r="D11" s="2">
-        <f>C11/1024</f>
+        <f t="shared" si="1"/>
         <v>0.92246138020418589</v>
       </c>
       <c r="F11" s="2">
@@ -2634,11 +5528,11 @@
         <v>841931924.28999996</v>
       </c>
       <c r="C12" s="2">
-        <f>B12/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>802.92885235786434</v>
       </c>
       <c r="D12" s="2">
-        <f>C12/1024</f>
+        <f t="shared" si="1"/>
         <v>0.7841102073807269</v>
       </c>
       <c r="F12" s="2">
@@ -2654,11 +5548,11 @@
         <v>759768734.27999997</v>
       </c>
       <c r="C13" s="2">
-        <f>B13/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>724.57192829132077</v>
       </c>
       <c r="D13" s="2">
-        <f>C13/1024</f>
+        <f t="shared" si="1"/>
         <v>0.70758977372199294</v>
       </c>
       <c r="F13" s="2">
@@ -2674,11 +5568,11 @@
         <v>718659309.32000005</v>
       </c>
       <c r="C14" s="2">
-        <f>B14/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>685.36692554473882</v>
       </c>
       <c r="D14" s="2">
-        <f>C14/1024</f>
+        <f t="shared" si="1"/>
         <v>0.669303638227284</v>
       </c>
       <c r="E14" s="2">
@@ -2695,11 +5589,11 @@
         <v>504073171.61000001</v>
       </c>
       <c r="C15" s="2">
-        <f>B15/(1024*1024)</f>
+        <f t="shared" si="0"/>
         <v>480.72163735389711</v>
       </c>
       <c r="D15" s="2">
-        <f>C15/1024</f>
+        <f t="shared" si="1"/>
         <v>0.46945472397841514</v>
       </c>
       <c r="E15" s="2">
@@ -2742,4 +5636,382 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D21D16B-2B11-4AFD-856B-7759E68D0D73}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1071404.2837357901</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1071404.2837357901</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6">
+        <v>140799.736055374</v>
+      </c>
+      <c r="D3" s="7">
+        <v>140799.736055374</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6">
+        <v>92102.826735690702</v>
+      </c>
+      <c r="D4" s="6">
+        <v>92102.826735690702</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6">
+        <v>50613.656070507001</v>
+      </c>
+      <c r="D5" s="10">
+        <v>50613.656070507001</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43155.413311345597</v>
+      </c>
+      <c r="D6" s="9">
+        <v>43155.413311345597</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1942.3214943963001</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1942.3214943963001</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E10F63-B14C-4D5B-85E5-B188C1E7E948}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1189729.9471072999</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1189729.9471072999</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6">
+        <v>143090.62753517399</v>
+      </c>
+      <c r="D3" s="7">
+        <v>143090.62753517399</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6">
+        <v>76214.313856519497</v>
+      </c>
+      <c r="D4" s="11">
+        <v>76214.313856519497</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6">
+        <v>44284.941270658899</v>
+      </c>
+      <c r="D5" s="8">
+        <v>44284.941270658899</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="6">
+        <v>42861.6945536434</v>
+      </c>
+      <c r="D6" s="11">
+        <v>42861.6945536434</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2751.1005385550702</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2751.1005385550702</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1189729.9471072999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="8">
+        <v>143090.62753517399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="8">
+        <v>76214.313856519497</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="8">
+        <v>44284.941270658899</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="8">
+        <v>42861.6945536434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2751.1005385550702</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>